<commit_message>
Agregando api para listar usuarios
</commit_message>
<xml_diff>
--- a/doc/operations.xlsx
+++ b/doc/operations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{BDB7EF1B-B826-A641-9382-9F930F09E1D8}"/>
+    <workbookView xWindow="5560" yWindow="2980" windowWidth="28040" windowHeight="17440" xr2:uid="{BDB7EF1B-B826-A641-9382-9F930F09E1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
   <si>
     <t xml:space="preserve">Operaciones necesarias </t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>listar organizaciones</t>
+  </si>
+  <si>
+    <t>obtener detalles</t>
   </si>
 </sst>
 </file>
@@ -619,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34D31FA-4219-3B44-A4ED-A01CE3287F3A}">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="139" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="139" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,8 +736,8 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3">
-        <f>AVERAGE(D16:D26)</f>
-        <v>27.375</v>
+        <f>AVERAGE(D16:D27)</f>
+        <v>46.555555555555557</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -755,47 +758,47 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
       <c r="D20" s="1">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>71</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -803,116 +806,116 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>74</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3">
-        <f>AVERAGE(D28:D45)</f>
-        <v>40.714285714285715</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3">
+        <f>AVERAGE(D29:D47)</f>
+        <v>53.333333333333336</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>4</v>
+      <c r="C31" t="s">
+        <v>8</v>
       </c>
       <c r="D31" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D37" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="1">
-        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -920,7 +923,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40" s="1">
         <v>100</v>
@@ -928,7 +931,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -936,133 +939,133 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D42" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="1">
-        <v>70</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D46" s="1">
+        <v>100</v>
+      </c>
+      <c r="E46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3">
-        <f>AVERAGE(D47:D50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3">
+        <f>AVERAGE(D49:D52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C48" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
         <v>20</v>
       </c>
-      <c r="D49" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="3">
-        <f>AVERAGE(D52:D60)</f>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3">
+        <f>AVERAGE(D54:D62)</f>
         <v>14.285714285714286</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C53" t="s">
-        <v>22</v>
-      </c>
-      <c r="D53" s="1">
-        <v>50</v>
-      </c>
-      <c r="E53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
-        <v>23</v>
-      </c>
-      <c r="D54" s="1">
-        <v>50</v>
-      </c>
-      <c r="E54" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D55" s="1">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="E55" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>26</v>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="1">
+        <v>50</v>
+      </c>
+      <c r="E56" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C58" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="1">
-        <v>0</v>
+      <c r="B58" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -1070,84 +1073,84 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>42</v>
+      <c r="C61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C63" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" s="1">
-        <v>0</v>
+      <c r="B63" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="3">
-        <f>AVERAGE(D68:D78)</f>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="3">
+        <f>AVERAGE(D70:D80)</f>
         <v>18.75</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C68" t="s">
-        <v>54</v>
-      </c>
-      <c r="D68" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
-        <v>57</v>
-      </c>
-      <c r="D69" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D70" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D71" s="1">
         <v>0</v>
@@ -1155,7 +1158,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D72" s="1">
         <v>0</v>
@@ -1163,7 +1166,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -1171,18 +1174,15 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D74" s="1">
-        <v>50</v>
-      </c>
-      <c r="E74" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -1190,61 +1190,64 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="1">
+        <v>50</v>
+      </c>
+      <c r="E76" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>58</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
         <v>19</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D81" s="1">
         <v>50</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C80" t="s">
-        <v>56</v>
-      </c>
-      <c r="D80" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
-        <v>61</v>
-      </c>
-      <c r="D83" s="1">
-        <v>0</v>
+      <c r="B83" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D84" s="1">
         <v>0</v>
@@ -1252,64 +1255,64 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
+        <v>61</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
         <v>63</v>
       </c>
-      <c r="D85" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
         <v>19</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D91" s="1">
         <v>50</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
-        <v>56</v>
-      </c>
-      <c r="D90" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C93" t="s">
-        <v>61</v>
-      </c>
-      <c r="D93" s="1">
-        <v>0</v>
+      <c r="B93" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D94" s="1">
         <v>0</v>
@@ -1317,7 +1320,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D95" s="1">
         <v>0</v>
@@ -1325,72 +1328,72 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D96" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
-        <v>42</v>
+      <c r="C97" t="s">
+        <v>63</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C98" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D98" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
-        <v>73</v>
-      </c>
-      <c r="D99" s="1">
-        <v>0</v>
+      <c r="B99" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C100" t="s">
+        <v>72</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>73</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
         <v>74</v>
       </c>
-      <c r="D100" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
+      <c r="D102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B103" t="s">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C104" t="s">
-        <v>68</v>
-      </c>
-      <c r="D104" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C105" t="s">
-        <v>67</v>
-      </c>
-      <c r="D105" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C106" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D106" s="1">
         <v>0</v>
@@ -1398,7 +1401,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D107" s="1">
         <v>0</v>
@@ -1406,14 +1409,30 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
+        <v>69</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
         <v>71</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D110" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D4:D87 D96:D1013">
+  <conditionalFormatting sqref="D4:D89 D98:D1015">
     <cfRule type="iconSet" priority="6">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
@@ -1423,7 +1442,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D88:D95">
+  <conditionalFormatting sqref="D90:D97">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>

</xml_diff>